<commit_message>
Added saving test result for each data from DataProvider
</commit_message>
<xml_diff>
--- a/GitHubTest/xls/TestCases.xlsx
+++ b/GitHubTest/xls/TestCases.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="TestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Test case</t>
   </si>
@@ -71,9 +71,6 @@
     <t>2. Click the notifications icon, check that all sections present</t>
   </si>
   <si>
-    <t>Passed</t>
-  </si>
-  <si>
     <t>3. testNotifications</t>
   </si>
   <si>
@@ -111,13 +108,22 @@
   </si>
   <si>
     <t>3. Delete repository, check that message about successful deleting appeared and check that name of deleted repository is not presented</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>!@[]\#^</t>
+  </si>
+  <si>
+    <t>Expected result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +134,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,18 +204,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,16 +548,14 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -549,9 +564,7 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -560,9 +573,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -571,9 +582,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -582,22 +591,18 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -606,22 +611,18 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -630,16 +631,14 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -648,7 +647,7 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -657,7 +656,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -666,7 +665,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -675,7 +674,7 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -683,10 +682,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -695,7 +694,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -704,7 +703,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -809,24 +808,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -836,18 +846,43 @@
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added using ChromeDriver to settings and method if click doesnt't work with ChromeDriver
</commit_message>
<xml_diff>
--- a/GitHubTest/xls/TestCases.xlsx
+++ b/GitHubTest/xls/TestCases.xlsx
@@ -521,7 +521,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +811,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +854,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added RepositoryAbstractPage class, test for checking issues creating
</commit_message>
<xml_diff>
--- a/GitHubTest/xls/TestCases.xlsx
+++ b/GitHubTest/xls/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Test case</t>
   </si>
@@ -80,9 +80,6 @@
     <t>1. testLogin</t>
   </si>
   <si>
-    <t>4. testRepositoryCreating</t>
-  </si>
-  <si>
     <t>1. Log in, check that button to create repository presents and click it</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>5. Delete this repository</t>
   </si>
   <si>
-    <t>5. testRepositoryDeleting</t>
-  </si>
-  <si>
     <t>1. Create new repository, go to settings</t>
   </si>
   <si>
@@ -117,6 +111,33 @@
   </si>
   <si>
     <t>Expected result</t>
+  </si>
+  <si>
+    <t>4. testAddRepository</t>
+  </si>
+  <si>
+    <t>5. testDeleteRepository</t>
+  </si>
+  <si>
+    <t>6. testAddIssue</t>
+  </si>
+  <si>
+    <t>2. Click on Issues link, check that all sections and welcome message present</t>
+  </si>
+  <si>
+    <t>3. Click the link to create issue, check that Title, Comments fields and Labels, Milestone, Assignee links present</t>
+  </si>
+  <si>
+    <t>4. Fill all fields and confirm creating, check that issue submitted</t>
+  </si>
+  <si>
+    <t>5. Navigate to Issues Section page and check that new issue appeared in the list of issues</t>
+  </si>
+  <si>
+    <t>6. Delete repository</t>
+  </si>
+  <si>
+    <t>1. Log in, add new repository</t>
   </si>
 </sst>
 </file>
@@ -520,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,10 +656,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -647,7 +668,7 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -656,7 +677,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -665,7 +686,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -674,7 +695,7 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -682,10 +703,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -694,7 +715,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -703,50 +724,64 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -810,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -861,7 +896,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
@@ -871,7 +906,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>13</v>

</xml_diff>